<commit_message>
Updated Code for Robot Task2 Control
</commit_message>
<xml_diff>
--- a/机器人点位映射关系.xlsx
+++ b/机器人点位映射关系.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Robotic\RoboticManipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1706C14-B43A-4580-A1EF-5D4617D600FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F70A601-68B9-472A-813E-186E054A8088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{CDDD5614-B249-45A2-B234-AC811943B192}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="31.25" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>